<commit_message>
bug fix: remove invalid characters of the file name that are not support in windows platform
</commit_message>
<xml_diff>
--- a/metadata_manager/output/apr_literature_metadata.xlsx
+++ b/metadata_manager/output/apr_literature_metadata.xlsx
@@ -1239,12 +1239,12 @@
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
         <is>
-          <t>['Java', ' Python']</t>
+          <t>['Java', 'Python']</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>['Defects4J', ' QuixBugs', ' ConDefects']</t>
+          <t>['Defects4J', 'QuixBugs', 'ConDefects']</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -3919,7 +3919,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Automated Program Repair via Conversation: Fixing 162 out of 337 Bugs for \$0.42 Each using ChatGPT</t>
+          <t>Automated program repair via conversation: Fixing 162 out of 337 bugs for $0.42 each using chatgpt</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -3968,7 +3968,7 @@
       <c r="L44" t="inlineStr">
         <is>
           <t>@inproceedings{xia2024automated,
-  title={Automated Program Repair via Conversation: Fixing 162 out of 337 Bugs for \$0.42 Each using ChatGPT},
+  title={Automated program repair via conversation: Fixing 162 out of 337 bugs for $0.42 each using chatgpt},
   author={Xia, Chunqiu Steven and Zhang, Lingming},
   booktitle={Proceedings of the 33rd ACM SIGSOFT International Symposium on Software Testing and Analysis},
   pages={819--831},

</xml_diff>